<commit_message>
Removed send song option from searchVC. Fixed crash in friendsVC searchDisplayController tableView by creating initializer methods for suggestion and request button arrays (instead of lazily instantiating). Change searchVC appearance - white background, blue search button, larger autocomplete table cells, and activity indicator for autocomplete results. Sent and received links art now loaded on low priority queues. Deleted commented out UIWebView JavaScript code for autoplay behavior in searchResultsVC.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="41340" yWindow="0" windowWidth="22600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="39740" yWindow="0" windowWidth="22600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="351">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -772,9 +772,6 @@
   </si>
   <si>
     <t>Use of IS_IOS8 macro</t>
-  </si>
-  <si>
-    <t>Rotation constants rewritten with #define</t>
   </si>
   <si>
     <t>Use of IS_IPHONE5 macro (lack of IS_IPHONE6)</t>
@@ -944,18 +941,12 @@
     <t>Added "find friends" to signup flow; created linkWithFB VC; registered as LLC with SoS</t>
   </si>
   <si>
-    <t>Loading indicator on "select video" screen</t>
-  </si>
-  <si>
     <t>Advertising: AppInstalls, HackerNews, etc.</t>
   </si>
   <si>
     <t>Refresh expired FB access tokens</t>
   </si>
   <si>
-    <t>Ask for push notif permissions again if denied</t>
-  </si>
-  <si>
     <t>Friends VC search - accepted request</t>
   </si>
   <si>
@@ -1023,12 +1014,6 @@
   </si>
   <si>
     <t>Met with Devansh</t>
-  </si>
-  <si>
-    <t>Link message invites via texts/FB message</t>
-  </si>
-  <si>
-    <t>Address book (phone contacts) integration</t>
   </si>
   <si>
     <t>Deleting links and friend requests</t>
@@ -1124,9 +1109,6 @@
     <t>Other content sources (i.e. Soundcloud)</t>
   </si>
   <si>
-    <t>Friends list options (alphabetical, best friends)</t>
-  </si>
-  <si>
     <t>Monday (5/25)</t>
   </si>
   <si>
@@ -1201,6 +1183,9 @@
   </si>
   <si>
     <t>Photoshop - $10</t>
+  </si>
+  <si>
+    <t>App invites</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1360,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1841">
+  <cellStyleXfs count="1863">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3248,7 +3255,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1841">
+  <cellStyles count="1863">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4169,6 +4176,17 @@
     <cellStyle name="Followed Hyperlink" xfId="1836" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1838" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1862" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5089,6 +5107,17 @@
     <cellStyle name="Hyperlink" xfId="1835" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1837" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1861" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5423,8 +5452,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5453,7 +5482,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -5471,10 +5500,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>350</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5485,19 +5514,19 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="24" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>313</v>
+      <c r="C5" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="24" t="s">
-        <v>324</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>323</v>
+        <v>316</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5507,11 +5536,11 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>315</v>
+      <c r="C7" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D7" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5524,8 +5553,8 @@
       <c r="C8" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="D8" t="s">
-        <v>333</v>
+      <c r="D8" s="9" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5533,13 +5562,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>121</v>
+        <v>322</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5549,11 +5578,8 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="23" t="s">
-        <v>334</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
+      <c r="C10" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5563,8 +5589,8 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>150</v>
+      <c r="C11" s="20" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5574,9 +5600,6 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
@@ -5586,14 +5609,20 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>134</v>
+      <c r="C13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="20" t="s">
-        <v>205</v>
+      <c r="C14" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>326</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -5604,6 +5633,12 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
+      <c r="C15" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5">
@@ -5613,11 +5648,11 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
+      <c r="C16" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>170</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5628,11 +5663,11 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>331</v>
+      <c r="C17" t="s">
+        <v>287</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5642,11 +5677,11 @@
       <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>135</v>
+      <c r="C18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>130</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -5657,11 +5692,11 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>244</v>
+      <c r="C19" s="20" t="s">
+        <v>245</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>48</v>
       </c>
       <c r="E19" s="13"/>
     </row>
@@ -5673,10 +5708,10 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>290</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5686,20 +5721,17 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>130</v>
+      <c r="C21" s="5" t="s">
+        <v>161</v>
       </c>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="C22" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
+      <c r="C22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -5710,11 +5742,11 @@
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
+      <c r="C23" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -5726,7 +5758,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="E24" s="13"/>
     </row>
@@ -5737,12 +5769,6 @@
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>128</v>
-      </c>
       <c r="E25" s="12"/>
     </row>
     <row r="26" spans="1:5">
@@ -5752,11 +5778,11 @@
       <c r="B26" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>182</v>
+      <c r="C26" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="E26" s="11"/>
     </row>
@@ -5767,8 +5793,11 @@
       <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>168</v>
+      <c r="C27" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5778,6 +5807,12 @@
       <c r="B28" t="s">
         <v>98</v>
       </c>
+      <c r="C28" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
       <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5">
@@ -5787,20 +5822,17 @@
       <c r="B29" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>164</v>
+      <c r="C29" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29" t="s">
+        <v>166</v>
       </c>
       <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="C30" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>353</v>
+      <c r="D30" t="s">
+        <v>338</v>
       </c>
       <c r="E30" s="11"/>
     </row>
@@ -5811,11 +5843,11 @@
       <c r="B31" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="24" t="s">
-        <v>322</v>
+      <c r="C31" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5825,11 +5857,11 @@
       <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>247</v>
+      <c r="C32" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -5840,8 +5872,11 @@
       <c r="B33" t="s">
         <v>99</v>
       </c>
+      <c r="C33" s="7" t="s">
+        <v>143</v>
+      </c>
       <c r="D33" t="s">
-        <v>344</v>
+        <v>197</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -5852,11 +5887,8 @@
       <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D34" t="s">
-        <v>199</v>
+      <c r="C34" t="s">
+        <v>217</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -5867,11 +5899,11 @@
       <c r="B35" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="D35" t="s">
-        <v>196</v>
+      <c r="C35" t="s">
+        <v>237</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="E35" s="14"/>
     </row>
@@ -5882,11 +5914,11 @@
       <c r="B36" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D36" t="s">
-        <v>197</v>
+      <c r="C36" t="s">
+        <v>299</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="E36" s="11"/>
     </row>
@@ -5898,16 +5930,19 @@
         <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>217</v>
+        <v>311</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
       <c r="C38" t="s">
-        <v>237</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>242</v>
+        <v>349</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="E38" s="12"/>
     </row>
@@ -5918,11 +5953,8 @@
       <c r="B39" t="s">
         <v>65</v>
       </c>
-      <c r="C39" t="s">
-        <v>302</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>238</v>
+      <c r="D39" s="22" t="s">
+        <v>252</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -5934,10 +5966,10 @@
         <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -5949,10 +5981,10 @@
         <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>355</v>
+        <v>298</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="E41" s="11"/>
     </row>
@@ -5963,8 +5995,11 @@
       <c r="B42" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="22" t="s">
-        <v>253</v>
+      <c r="C42" t="s">
+        <v>297</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="E42" s="11"/>
     </row>
@@ -5975,11 +6010,8 @@
       <c r="B43" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C43" t="s">
-        <v>299</v>
-      </c>
       <c r="D43" s="4" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="E43" s="17"/>
     </row>
@@ -5991,10 +6023,7 @@
         <v>140</v>
       </c>
       <c r="C44" t="s">
-        <v>301</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>241</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6005,17 +6034,11 @@
         <v>141</v>
       </c>
       <c r="C45" t="s">
-        <v>300</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>243</v>
+        <v>324</v>
       </c>
       <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="D46" s="4" t="s">
-        <v>239</v>
-      </c>
       <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5">
@@ -6025,12 +6048,6 @@
       <c r="B47" t="s">
         <v>77</v>
       </c>
-      <c r="C47" t="s">
-        <v>328</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>273</v>
-      </c>
       <c r="E47" s="17"/>
     </row>
     <row r="48" spans="1:5">
@@ -6040,9 +6057,6 @@
       <c r="B48" t="s">
         <v>79</v>
       </c>
-      <c r="C48" t="s">
-        <v>329</v>
-      </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
@@ -6522,7 +6536,7 @@
         <v>229</v>
       </c>
       <c r="B118" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -6559,7 +6573,7 @@
         <v>236</v>
       </c>
       <c r="B124" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -6572,275 +6586,275 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B128" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
+        <v>256</v>
+      </c>
+      <c r="B130" t="s">
         <v>257</v>
-      </c>
-      <c r="B130" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B131" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134" t="s">
         <v>260</v>
-      </c>
-      <c r="B134" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
+        <v>261</v>
+      </c>
+      <c r="B135" t="s">
         <v>262</v>
-      </c>
-      <c r="B135" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" t="s">
         <v>264</v>
-      </c>
-      <c r="B136" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
+        <v>267</v>
+      </c>
+      <c r="B137" t="s">
         <v>268</v>
-      </c>
-      <c r="B137" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
+        <v>265</v>
+      </c>
+      <c r="B139" t="s">
         <v>266</v>
-      </c>
-      <c r="B139" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B143" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
+        <v>275</v>
+      </c>
+      <c r="B144" t="s">
         <v>276</v>
-      </c>
-      <c r="B144" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
+        <v>277</v>
+      </c>
+      <c r="B145" t="s">
         <v>278</v>
-      </c>
-      <c r="B145" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
+        <v>279</v>
+      </c>
+      <c r="B146" t="s">
         <v>280</v>
-      </c>
-      <c r="B146" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B149" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B150" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B153" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B158" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B159" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B161" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B163" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B164" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B167" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B168" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B169" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B170" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B171" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B172" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="8" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed push notification screenshot to image of badged app icon. Redesigned searchVC - introduced magnifying glass icon and caption (to replace videoPromptLabel), moved search bar to top of view and enabled gray background, and eliminated search bar button. Animated new searchVC content (icon/caption) on search bar click, and handled special cases. Introduced methods -resetScreenContents and -animateScreenContentsInDirection. Changed tap gesture recognition code in searchVC, making autocomplete entries easier to select (now searchDisplayController is dismissed only if touch lands in header). Addressed bug in contactsVC sendLink button animation by animating constraint instead of frame. Addressed bug in contactsVC "Recents" section by creating new contactAndState dictionary for user if "LMU Users" section present. Replaced dataWithContentsOfURL with NSURLSession dataTaskWithURL in Data.m, significantly improving link load times on iPhone 6.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39740" yWindow="0" windowWidth="22600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="38700" yWindow="1880" windowWidth="25040" windowHeight="20180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="362">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Simultaneous friend requests</t>
   </si>
   <si>
-    <t>Alternatives to EchoNest</t>
-  </si>
-  <si>
     <t>Alternatives to Parse</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>move loadUpdatedLink, etc. to superclass</t>
   </si>
   <si>
-    <t>move local data update functions to data model</t>
-  </si>
-  <si>
     <t>Periodic data updates, data/memory usage tests, link VC song header, iTunes cell</t>
   </si>
   <si>
@@ -609,9 +603,6 @@
     <t>Song search behavior, update timer bug, set up iPhone 5s, XIB files autolayout</t>
   </si>
   <si>
-    <t>use programmatically created UISearchBar</t>
-  </si>
-  <si>
     <t>use opaque bottom bar setting in XIB files</t>
   </si>
   <si>
@@ -757,12 +748,6 @@
   </si>
   <si>
     <t>UIWebView autoplay failures</t>
-  </si>
-  <si>
-    <t>Testing/Marketing</t>
-  </si>
-  <si>
-    <t>Read about TestFlight beta testing program</t>
   </si>
   <si>
     <t>Fall Break</t>
@@ -941,9 +926,6 @@
     <t>Added "find friends" to signup flow; created linkWithFB VC; registered as LLC with SoS</t>
   </si>
   <si>
-    <t>Advertising: AppInstalls, HackerNews, etc.</t>
-  </si>
-  <si>
     <t>Refresh expired FB access tokens</t>
   </si>
   <si>
@@ -1029,18 +1011,6 @@
   </si>
   <si>
     <t>Continue playing audio in BG w/o interruption</t>
-  </si>
-  <si>
-    <t>Single search option</t>
-  </si>
-  <si>
-    <t>Consistent color scheme</t>
-  </si>
-  <si>
-    <t>Screenshot captions in App Store</t>
-  </si>
-  <si>
-    <t>Favorite links/send to self</t>
   </si>
   <si>
     <t>Received vs. sent tab bar colors</t>
@@ -1100,9 +1070,6 @@
     <t>Sunday (5/24)</t>
   </si>
   <si>
-    <t>Links loading slow on app launch</t>
-  </si>
-  <si>
     <t>Updated to Xcode 6.3; resolved 2 GTL YT errors</t>
   </si>
   <si>
@@ -1182,10 +1149,76 @@
     <t>Selection of autocomplete entries</t>
   </si>
   <si>
-    <t>Photoshop - $10</t>
-  </si>
-  <si>
     <t>App invites</t>
+  </si>
+  <si>
+    <t>Search bar / VC appearance</t>
+  </si>
+  <si>
+    <t>move local data update functions out of Data.m</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t>A/B Testing</t>
+  </si>
+  <si>
+    <t>Crash/Bug Reports</t>
+  </si>
+  <si>
+    <t>Before Shipping</t>
+  </si>
+  <si>
+    <t>Remove trunk/Examples and build/</t>
+  </si>
+  <si>
+    <t>Analytics - Apple, Parse</t>
+  </si>
+  <si>
+    <t>Favorite links</t>
+  </si>
+  <si>
+    <t>Links loading slow on app launch / blocks UI</t>
+  </si>
+  <si>
+    <t>Marketing/Release</t>
+  </si>
+  <si>
+    <t>App Store keywords and Google meta tags</t>
+  </si>
+  <si>
+    <t>Submit to app review sites</t>
+  </si>
+  <si>
+    <t>New screenshots and App Store description</t>
+  </si>
+  <si>
+    <t>Screenshot frames and captions</t>
+  </si>
+  <si>
+    <t>Post on news site and public forums</t>
+  </si>
+  <si>
+    <t>Android Development</t>
+  </si>
+  <si>
+    <t>Interview/hire Android developer</t>
+  </si>
+  <si>
+    <t>List of features/bug fixes to implement</t>
+  </si>
+  <si>
+    <t>Test Android app build on another computer</t>
+  </si>
+  <si>
+    <t>Test LMU app build on another computer</t>
+  </si>
+  <si>
+    <t>Launch Screen - $7</t>
+  </si>
+  <si>
+    <t>Photoshop - $20</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1346,6 +1379,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC4D79B"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -1360,7 +1399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1863">
+  <cellStyleXfs count="1967">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3224,8 +3263,112 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3251,11 +3394,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1863">
+  <cellStyles count="1967">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4187,6 +4331,58 @@
     <cellStyle name="Followed Hyperlink" xfId="1858" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1860" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1878" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1880" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1882" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1884" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1886" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1888" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1890" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1892" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1894" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1896" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1898" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1900" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1902" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1904" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1906" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1908" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1910" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1912" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1914" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1916" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1918" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1920" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1922" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1924" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1932" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1934" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1936" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1938" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1958" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1960" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1962" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1964" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1966" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5118,6 +5314,58 @@
     <cellStyle name="Hyperlink" xfId="1857" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1859" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1877" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1879" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1881" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1883" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1885" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1887" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1889" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1891" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1893" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1895" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1897" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1899" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1901" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1903" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1905" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1907" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1909" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1911" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1913" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1915" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1917" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1919" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1921" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1923" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1931" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1933" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1935" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1937" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1957" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1959" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1961" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1963" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1965" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5452,8 +5700,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5482,13 +5730,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -5500,10 +5748,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>350</v>
+        <v>339</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>338</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5514,19 +5762,19 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>318</v>
+      <c r="C5" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="24" t="s">
-        <v>316</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>310</v>
+      <c r="C6" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5536,11 +5784,11 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D7" t="s">
-        <v>328</v>
+      <c r="C7" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5550,11 +5798,11 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>121</v>
+      <c r="C8" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5562,10 +5810,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -5578,8 +5826,8 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>134</v>
+      <c r="C10" s="20" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5589,9 +5837,6 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -5600,6 +5845,12 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
@@ -5609,20 +5860,20 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
+      <c r="C13" s="27" t="s">
+        <v>307</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>348</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="23" t="s">
-        <v>313</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>326</v>
+      <c r="C14" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -5633,11 +5884,11 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>135</v>
+      <c r="C15" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" t="s">
+        <v>168</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -5648,11 +5899,11 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>244</v>
+      <c r="C16" t="s">
+        <v>281</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5663,11 +5914,11 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" t="s">
-        <v>287</v>
+      <c r="C17" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5675,13 +5926,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="D18" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -5692,11 +5943,8 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="D19" t="s">
-        <v>48</v>
+      <c r="C19" t="s">
+        <v>126</v>
       </c>
       <c r="E19" s="13"/>
     </row>
@@ -5707,11 +5955,8 @@
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
+      <c r="C20" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5722,16 +5967,19 @@
         <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>161</v>
+        <v>84</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
       <c r="C22" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>128</v>
+        <v>215</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -5743,10 +5991,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -5757,9 +6002,6 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5">
@@ -5767,7 +6009,13 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>344</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -5776,28 +6024,27 @@
         <v>36</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E26" s="11"/>
+        <v>96</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>353</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5805,49 +6052,46 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>317</v>
-      </c>
-      <c r="D28" t="s">
-        <v>165</v>
-      </c>
-      <c r="E28" s="11"/>
+        <v>350</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D29" t="s">
-        <v>166</v>
-      </c>
-      <c r="E29" s="11"/>
+        <v>56</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="D30" t="s">
-        <v>338</v>
-      </c>
-      <c r="E30" s="11"/>
+      <c r="C30" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>177</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" t="s">
-        <v>199</v>
+        <v>175</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5855,1012 +6099,1045 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="D32" t="s">
-        <v>196</v>
+        <v>57</v>
       </c>
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" t="s">
-        <v>197</v>
+        <v>98</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>217</v>
+        <v>58</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>336</v>
       </c>
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" t="s">
-        <v>237</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>242</v>
+        <v>59</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="D35" t="s">
+        <v>164</v>
       </c>
       <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>299</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>238</v>
+        <v>60</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="D36" t="s">
+        <v>340</v>
       </c>
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" t="s">
-        <v>311</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>251</v>
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>327</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="C38" t="s">
-        <v>349</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>250</v>
+      <c r="D38" t="s">
+        <v>196</v>
       </c>
       <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>252</v>
+        <v>64</v>
+      </c>
+      <c r="D39" t="s">
+        <v>194</v>
       </c>
       <c r="E39" s="17"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" t="s">
-        <v>296</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>241</v>
+        <v>68</v>
       </c>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" t="s">
-        <v>298</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>243</v>
+        <v>94</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" t="s">
-        <v>297</v>
+        <v>69</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C44" t="s">
-        <v>323</v>
+        <v>214</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>324</v>
+        <v>234</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5">
+      <c r="C46" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>238</v>
+      </c>
       <c r="E46" s="17"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" t="s">
         <v>76</v>
       </c>
-      <c r="B47" t="s">
-        <v>77</v>
+      <c r="C47" t="s">
+        <v>305</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>240</v>
       </c>
       <c r="E47" s="17"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
         <v>78</v>
       </c>
-      <c r="B48" t="s">
-        <v>79</v>
+      <c r="C48" t="s">
+        <v>360</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s">
         <v>80</v>
       </c>
-      <c r="B49" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="19"/>
+      <c r="C49" t="s">
+        <v>361</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
         <v>82</v>
       </c>
-      <c r="B50" t="s">
-        <v>83</v>
-      </c>
+      <c r="D50" s="19"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="C52" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B56" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" t="s">
         <v>101</v>
-      </c>
-      <c r="B58" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" t="s">
         <v>113</v>
-      </c>
-      <c r="B64" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" t="s">
         <v>118</v>
-      </c>
-      <c r="B67" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" t="s">
         <v>122</v>
-      </c>
-      <c r="B69" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" t="s">
         <v>146</v>
-      </c>
-      <c r="B79" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" t="s">
         <v>153</v>
-      </c>
-      <c r="B82" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" t="s">
         <v>157</v>
-      </c>
-      <c r="B84" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B87" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
+        <v>167</v>
+      </c>
+      <c r="B88" t="s">
         <v>169</v>
-      </c>
-      <c r="B88" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" t="s">
         <v>179</v>
-      </c>
-      <c r="B93" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B95" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B97" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B100" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B103" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B105" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B106" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="26" t="s">
-        <v>212</v>
+      <c r="A108" s="25" t="s">
+        <v>209</v>
       </c>
       <c r="B108" s="21"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B109" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B111" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B117" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B118" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B121" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B122" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B123" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B124" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B125" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B128" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B130" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B131" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B134" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B135" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B136" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B137" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B139" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B143" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B144" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B145" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B146" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B149" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B150" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B153" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B156" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B158" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B159" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B161" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="B163" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="B164" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B167" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B168" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B169" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B170" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B171" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="B172" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="8" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="24" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Replaced all (active) instances of dataWithContentsOfURL and NSURLConnection with NSURLSession in searchVC, songInfoVC, and searchResultsVC. Reverted to repeating, 10 second interval updates for Badge push notification setting.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38700" yWindow="1880" windowWidth="25040" windowHeight="20180" tabRatio="500"/>
+    <workbookView xWindow="39980" yWindow="0" windowWidth="21740" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="360">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -408,9 +408,6 @@
     <t>Thursday (8/7)</t>
   </si>
   <si>
-    <t>Alternatives to NSURLConnection</t>
-  </si>
-  <si>
     <t>Added toolbar icons, customized YT search bar, back buttons, "sent to" field, play icon</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>Remove blank messages</t>
   </si>
   <si>
-    <t>Replace dataWithContentsOfURL?</t>
-  </si>
-  <si>
     <t>Saturday (8/9)</t>
   </si>
   <si>
@@ -523,9 +517,6 @@
   </si>
   <si>
     <t>Wednesday (8/20)</t>
-  </si>
-  <si>
-    <t>Song data caching w/time stamps?</t>
   </si>
   <si>
     <t>Moved iTunes cell, preview/available labels, streaming with AVPlayer</t>
@@ -1146,15 +1137,9 @@
     <t>declare dictionary keys as constants</t>
   </si>
   <si>
-    <t>Selection of autocomplete entries</t>
-  </si>
-  <si>
     <t>App invites</t>
   </si>
   <si>
-    <t>Search bar / VC appearance</t>
-  </si>
-  <si>
     <t>move local data update functions out of Data.m</t>
   </si>
   <si>
@@ -1179,9 +1164,6 @@
     <t>Favorite links</t>
   </si>
   <si>
-    <t>Links loading slow on app launch / blocks UI</t>
-  </si>
-  <si>
     <t>Marketing/Release</t>
   </si>
   <si>
@@ -1219,6 +1201,18 @@
   </si>
   <si>
     <t>Photoshop - $20</t>
+  </si>
+  <si>
+    <t>Autocomplete results table scroll</t>
+  </si>
+  <si>
+    <t>SearchResultsVC table animation (iOS 8)</t>
+  </si>
+  <si>
+    <t>Using file system cache to improve link load time</t>
+  </si>
+  <si>
+    <t>InboxVC paging</t>
   </si>
 </sst>
 </file>
@@ -1399,8 +1393,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1967">
+  <cellStyleXfs count="1979">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3399,7 +3405,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1967">
+  <cellStyles count="1979">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4383,6 +4389,12 @@
     <cellStyle name="Followed Hyperlink" xfId="1962" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1964" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1966" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1968" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1970" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1972" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1974" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1978" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5366,6 +5378,12 @@
     <cellStyle name="Hyperlink" xfId="1961" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1963" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1965" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1967" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1969" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1971" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1973" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1977" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5700,8 +5718,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5730,7 +5748,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -5747,11 +5765,11 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>339</v>
+      <c r="C4" s="23" t="s">
+        <v>356</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5762,16 +5780,16 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>337</v>
+      <c r="C5" s="10" t="s">
+        <v>357</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="10" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>120</v>
@@ -5785,10 +5803,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5799,10 +5817,10 @@
         <v>43</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5810,10 +5828,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -5827,7 +5845,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5861,19 +5879,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>307</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>348</v>
+        <v>304</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="C14" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>134</v>
+        <v>277</v>
+      </c>
+      <c r="D14" t="s">
+        <v>359</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -5885,10 +5903,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -5900,10 +5918,10 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D16" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5917,9 +5935,6 @@
       <c r="C17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="s">
-        <v>129</v>
-      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
@@ -5929,10 +5944,7 @@
         <v>63</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="D18" t="s">
-        <v>48</v>
+        <v>239</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -5946,6 +5958,7 @@
       <c r="C19" t="s">
         <v>126</v>
       </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5">
@@ -5956,7 +5969,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5976,10 +5989,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="C22" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -5991,7 +6004,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -6012,10 +6025,10 @@
         <v>54</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -6027,10 +6040,10 @@
         <v>96</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6041,10 +6054,10 @@
         <v>55</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6055,10 +6068,10 @@
         <v>97</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6069,18 +6082,18 @@
         <v>56</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="24" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6088,10 +6101,10 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6111,10 +6124,10 @@
         <v>98</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -6126,10 +6139,10 @@
         <v>58</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -6141,10 +6154,10 @@
         <v>59</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E35" s="14"/>
     </row>
@@ -6156,10 +6169,10 @@
         <v>60</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D36" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E36" s="11"/>
     </row>
@@ -6171,13 +6184,13 @@
         <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
       <c r="D38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E38" s="12"/>
     </row>
@@ -6189,7 +6202,7 @@
         <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -6210,10 +6223,10 @@
         <v>94</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E41" s="11"/>
     </row>
@@ -6225,10 +6238,10 @@
         <v>69</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E42" s="11"/>
     </row>
@@ -6240,10 +6253,10 @@
         <v>73</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E43" s="17"/>
     </row>
@@ -6252,13 +6265,13 @@
         <v>72</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6266,22 +6279,22 @@
         <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E46" s="17"/>
     </row>
@@ -6293,10 +6306,10 @@
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E47" s="17"/>
     </row>
@@ -6308,10 +6321,10 @@
         <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6322,10 +6335,10 @@
         <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6345,7 +6358,7 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6356,7 +6369,7 @@
         <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6367,7 +6380,7 @@
         <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6378,7 +6391,7 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -6389,7 +6402,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6461,7 +6474,7 @@
         <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -6493,7 +6506,7 @@
         <v>124</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -6501,7 +6514,7 @@
         <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -6509,629 +6522,629 @@
         <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>135</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B76" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B79" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B80" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B83" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B88" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B91" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" t="s">
         <v>185</v>
-      </c>
-      <c r="B96" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" t="s">
         <v>186</v>
-      </c>
-      <c r="B97" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B104" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="25" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B108" s="21"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B111" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B117" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B118" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B122" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B123" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B124" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B128" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B130" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B131" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B134" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B135" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B136" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B137" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B139" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B143" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B144" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B145" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B146" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B149" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B150" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B153" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B155" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B156" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B158" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B159" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B161" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B163" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B164" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B167" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B168" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B169" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B170" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B171" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B172" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved annotation to beginning of text message link (in front of URL). Removed condition on App Store link (now always included). Created Employment Contract.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39980" yWindow="0" windowWidth="21740" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="7200" yWindow="1540" windowWidth="19820" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t xml:space="preserve">Duplicate contents in self.userSearchContacts </t>
   </si>
   <si>
-    <t>*Push notifications</t>
-  </si>
-  <si>
     <t>Thursday (8/7)</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>Tried autoplay, VC transitions, art aspect fit, launch w/push notif, switch UISeg w/click on tab</t>
   </si>
   <si>
-    <t>Click on inbox tab should switch seg w/new push</t>
-  </si>
-  <si>
     <t>Link fetch before update, expanded receiversData, like/love with push notifs</t>
   </si>
   <si>
@@ -726,13 +720,7 @@
     <t>Sunday (11/2)</t>
   </si>
   <si>
-    <t>Horizontal table bounds animation (iOS 8)</t>
-  </si>
-  <si>
     <t>Hacks/Patches</t>
-  </si>
-  <si>
-    <t>Horizontal table position/separate VC (iOS 8)</t>
   </si>
   <si>
     <t>iTunes search special characters error</t>
@@ -1173,21 +1161,12 @@
     <t>Submit to app review sites</t>
   </si>
   <si>
-    <t>New screenshots and App Store description</t>
-  </si>
-  <si>
-    <t>Screenshot frames and captions</t>
-  </si>
-  <si>
     <t>Post on news site and public forums</t>
   </si>
   <si>
     <t>Android Development</t>
   </si>
   <si>
-    <t>Interview/hire Android developer</t>
-  </si>
-  <si>
     <t>List of features/bug fixes to implement</t>
   </si>
   <si>
@@ -1206,13 +1185,34 @@
     <t>Autocomplete results table scroll</t>
   </si>
   <si>
-    <t>SearchResultsVC table animation (iOS 8)</t>
-  </si>
-  <si>
     <t>Using file system cache to improve link load time</t>
   </si>
   <si>
     <t>InboxVC paging</t>
+  </si>
+  <si>
+    <t>Make contract/send to Sean Yu</t>
+  </si>
+  <si>
+    <t>searchResultsVC table frame + animation (iOS 8)</t>
+  </si>
+  <si>
+    <t>searchResultsVC - separate VC for iOS 8</t>
+  </si>
+  <si>
+    <t>Look into code review tool (git pull requests)</t>
+  </si>
+  <si>
+    <t>iOS 8 watch symbol</t>
+  </si>
+  <si>
+    <t>Send Link button label highlighting on click</t>
+  </si>
+  <si>
+    <t>Test whether UIImage imageWithData blocks UI</t>
+  </si>
+  <si>
+    <t>Clicking inbox tab should switch seg w/new push</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1393,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1979">
+  <cellStyleXfs count="2017">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3373,8 +3373,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3398,14 +3436,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1979">
+  <cellStyles count="2017">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4395,6 +4432,25 @@
     <cellStyle name="Followed Hyperlink" xfId="1974" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1976" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1998" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2016" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5384,6 +5440,25 @@
     <cellStyle name="Hyperlink" xfId="1973" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1975" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1997" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2013" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2015" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5718,8 +5793,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5748,7 +5823,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -5765,11 +5840,11 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>356</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>334</v>
+      <c r="C4" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>330</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5780,18 +5855,18 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>314</v>
+      <c r="C5" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>120</v>
       </c>
     </row>
@@ -5802,11 +5877,11 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>342</v>
+      <c r="C7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5816,11 +5891,11 @@
       <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>147</v>
+      <c r="C8" t="s">
+        <v>357</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5828,10 +5903,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>132</v>
+        <v>301</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -5844,8 +5919,8 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>199</v>
+      <c r="C10" s="4" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5855,6 +5930,9 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -5863,11 +5941,8 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>45</v>
+      <c r="C12" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="E12" s="5"/>
     </row>
@@ -5878,21 +5953,12 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>304</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>358</v>
+      <c r="C13" s="20" t="s">
+        <v>197</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="C14" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="D14" t="s">
-        <v>359</v>
-      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
@@ -5902,11 +5968,11 @@
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
+      <c r="C15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -5917,11 +5983,11 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
-        <v>278</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
+      <c r="C16" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>350</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -5932,8 +5998,11 @@
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>47</v>
+      <c r="C17" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5943,8 +6012,11 @@
       <c r="B18" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>239</v>
+      <c r="C18" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D18" t="s">
+        <v>351</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -5956,9 +6028,11 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="4"/>
+        <v>274</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:5">
@@ -5968,8 +6042,11 @@
       <c r="B20" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>158</v>
+      <c r="C20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5979,20 +6056,15 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>127</v>
-      </c>
+      <c r="C21" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="C22" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>177</v>
+      <c r="C22" t="s">
+        <v>126</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -6004,7 +6076,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -6015,6 +6087,10 @@
       <c r="B24" t="s">
         <v>33</v>
       </c>
+      <c r="C24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="6"/>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5">
@@ -6024,11 +6100,8 @@
       <c r="B25" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>339</v>
+      <c r="C25" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -6039,11 +6112,8 @@
       <c r="B26" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>347</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>341</v>
+      <c r="C26" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6053,12 +6123,6 @@
       <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>346</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
@@ -6067,11 +6131,11 @@
       <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>340</v>
+      <c r="C28" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6081,19 +6145,19 @@
       <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>345</v>
+      <c r="C29" s="23" t="s">
+        <v>340</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="C30" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="D30" s="26" t="s">
-        <v>336</v>
+      <c r="C30" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6101,10 +6165,13 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>337</v>
+        <v>171</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6114,6 +6181,9 @@
       <c r="B32" t="s">
         <v>57</v>
       </c>
+      <c r="D32" s="25" t="s">
+        <v>346</v>
+      </c>
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5">
@@ -6123,11 +6193,8 @@
       <c r="B33" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>161</v>
+      <c r="D33" s="25" t="s">
+        <v>336</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -6138,11 +6205,8 @@
       <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>333</v>
+      <c r="D34" s="25" t="s">
+        <v>332</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -6153,12 +6217,6 @@
       <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="28" t="s">
-        <v>352</v>
-      </c>
-      <c r="D35" t="s">
-        <v>162</v>
-      </c>
       <c r="E35" s="14"/>
     </row>
     <row r="36" spans="1:5">
@@ -6168,11 +6226,11 @@
       <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="D36" t="s">
-        <v>335</v>
+      <c r="C36" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="E36" s="11"/>
     </row>
@@ -6183,14 +6241,20 @@
       <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="D37" t="s">
-        <v>324</v>
+      <c r="C37" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>329</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
+      <c r="C38" s="10" t="s">
+        <v>355</v>
+      </c>
       <c r="D38" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="E38" s="12"/>
     </row>
@@ -6201,8 +6265,11 @@
       <c r="B39" t="s">
         <v>64</v>
       </c>
+      <c r="C39" s="10" t="s">
+        <v>344</v>
+      </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>331</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -6213,6 +6280,12 @@
       <c r="B40" t="s">
         <v>68</v>
       </c>
+      <c r="C40" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="D40" t="s">
+        <v>320</v>
+      </c>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5">
@@ -6222,11 +6295,8 @@
       <c r="B41" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>236</v>
+      <c r="D41" t="s">
+        <v>191</v>
       </c>
       <c r="E41" s="11"/>
     </row>
@@ -6237,11 +6307,8 @@
       <c r="B42" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>232</v>
+      <c r="D42" t="s">
+        <v>189</v>
       </c>
       <c r="E42" s="11"/>
     </row>
@@ -6252,12 +6319,6 @@
       <c r="B43" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>243</v>
-      </c>
       <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:5">
@@ -6265,13 +6326,13 @@
         <v>72</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" t="s">
-        <v>211</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>242</v>
+        <v>136</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6279,22 +6340,22 @@
         <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" t="s">
-        <v>231</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>244</v>
+        <v>137</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="C46" t="s">
-        <v>290</v>
+      <c r="C46" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E46" s="17"/>
     </row>
@@ -6306,10 +6367,10 @@
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>302</v>
+        <v>209</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E47" s="17"/>
     </row>
@@ -6321,10 +6382,10 @@
         <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>354</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6335,10 +6396,10 @@
         <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>355</v>
+        <v>286</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>264</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6348,7 +6409,12 @@
       <c r="B50" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="19"/>
+      <c r="C50" t="s">
+        <v>298</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
@@ -6358,7 +6424,10 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>287</v>
+        <v>347</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6369,7 +6438,7 @@
         <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6379,8 +6448,10 @@
       <c r="B53" t="s">
         <v>93</v>
       </c>
-      <c r="C53" t="s">
-        <v>288</v>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="C54" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6391,7 +6462,7 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -6402,7 +6473,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6420,6 +6491,9 @@
       <c r="B58" t="s">
         <v>101</v>
       </c>
+      <c r="C58" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="15" t="s">
@@ -6428,6 +6502,9 @@
       <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
+      <c r="C59" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="8" t="s">
@@ -6474,7 +6551,7 @@
         <v>115</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -6506,7 +6583,7 @@
         <v>124</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -6514,637 +6591,637 @@
         <v>125</v>
       </c>
       <c r="B72" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" t="s">
         <v>143</v>
-      </c>
-      <c r="B79" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
+        <v>149</v>
+      </c>
+      <c r="B82" t="s">
         <v>150</v>
-      </c>
-      <c r="B82" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
+        <v>153</v>
+      </c>
+      <c r="B84" t="s">
         <v>154</v>
-      </c>
-      <c r="B84" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
         <v>165</v>
-      </c>
-      <c r="B88" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" t="s">
         <v>167</v>
-      </c>
-      <c r="B89" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="15" t="s">
         <v>169</v>
-      </c>
-      <c r="B90" s="15" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B91" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B95" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B96" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B97" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B98" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
+        <v>194</v>
+      </c>
+      <c r="B103" t="s">
         <v>196</v>
-      </c>
-      <c r="B103" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B104" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
+        <v>199</v>
+      </c>
+      <c r="B105" t="s">
         <v>201</v>
-      </c>
-      <c r="B105" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B106" t="s">
         <v>202</v>
-      </c>
-      <c r="B106" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="25" t="s">
-        <v>206</v>
+      <c r="A108" s="24" t="s">
+        <v>204</v>
       </c>
       <c r="B108" s="21"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B109" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B111" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="B116" s="19" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B118" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B121" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B122" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
+        <v>225</v>
+      </c>
+      <c r="B123" t="s">
         <v>227</v>
-      </c>
-      <c r="B123" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B124" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B125" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B128" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B130" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B134" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B135" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B136" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B137" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B139" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B143" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B144" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B145" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B146" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B149" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B150" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B153" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B155" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B156" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B158" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B159" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B161" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B163" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B164" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B167" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B168" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B169" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B170" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B171" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B172" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="8" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LinkMeUp Version/Build 2.0 Archive
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1540" windowWidth="19820" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1191,9 +1191,6 @@
     <t>InboxVC paging</t>
   </si>
   <si>
-    <t>Make contract/send to Sean Yu</t>
-  </si>
-  <si>
     <t>searchResultsVC table frame + animation (iOS 8)</t>
   </si>
   <si>
@@ -1213,6 +1210,9 @@
   </si>
   <si>
     <t>Clicking inbox tab should switch seg w/new push</t>
+  </si>
+  <si>
+    <t>Send modified contract to Sean Yu</t>
   </si>
 </sst>
 </file>
@@ -5793,8 +5793,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5856,7 +5856,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>310</v>
@@ -5878,7 +5878,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>338</v>
@@ -5892,7 +5892,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>297</v>
@@ -5920,7 +5920,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6002,7 +6002,7 @@
         <v>273</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6242,7 +6242,7 @@
         <v>61</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>329</v>
@@ -6251,7 +6251,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="C38" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D38" t="s">
         <v>161</v>
@@ -6399,7 +6399,7 @@
         <v>286</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -7227,7 +7227,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="24" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Added Parse app LinkMeUp-Dev's keys to Constants.h App video (6/27 1:30 PM). Large media files excluded via gitignore.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8780" yWindow="3080" windowWidth="29220" windowHeight="19620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1082,9 +1082,6 @@
     <t>Saturday (5/30)</t>
   </si>
   <si>
-    <t>hold song/video data in NSDictionary</t>
-  </si>
-  <si>
     <t>Wrote todo list; researched/practiced git for Xcode</t>
   </si>
   <si>
@@ -1155,12 +1152,6 @@
     <t>Marketing/Release</t>
   </si>
   <si>
-    <t>App Store keywords and Google meta tags</t>
-  </si>
-  <si>
-    <t>Submit to app review sites</t>
-  </si>
-  <si>
     <t>Post on news site and public forums</t>
   </si>
   <si>
@@ -1170,18 +1161,12 @@
     <t>List of features/bug fixes to implement</t>
   </si>
   <si>
-    <t>Test Android app build on another computer</t>
-  </si>
-  <si>
     <t>Test LMU app build on another computer</t>
   </si>
   <si>
     <t>Launch Screen - $7</t>
   </si>
   <si>
-    <t>Photoshop - $20</t>
-  </si>
-  <si>
     <t>Autocomplete results table scroll</t>
   </si>
   <si>
@@ -1212,7 +1197,34 @@
     <t>Clicking inbox tab should switch seg w/new push</t>
   </si>
   <si>
-    <t>Send modified contract to Sean Yu</t>
+    <t>Google Apps - $5</t>
+  </si>
+  <si>
+    <t>Photoshop - $120</t>
+  </si>
+  <si>
+    <t>Build Android app on my computer</t>
+  </si>
+  <si>
+    <t>Contact journalists and app review sites</t>
+  </si>
+  <si>
+    <t>Beta testing</t>
+  </si>
+  <si>
+    <t>Develop app video</t>
+  </si>
+  <si>
+    <t>Settings/Privacy</t>
+  </si>
+  <si>
+    <t>Use saved address book if later denied</t>
+  </si>
+  <si>
+    <t>hold song/video data in NSDictionary (subclass?)</t>
+  </si>
+  <si>
+    <t>Web Hosting - $40 + $49</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1405,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2017">
+  <cellStyleXfs count="2049">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3411,8 +3423,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3441,8 +3485,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2017">
+  <cellStyles count="2049">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4451,6 +4496,22 @@
     <cellStyle name="Followed Hyperlink" xfId="2012" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2014" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2032" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2034" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2036" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2038" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2040" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2042" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2044" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2046" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2048" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5459,6 +5520,22 @@
     <cellStyle name="Hyperlink" xfId="2011" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2013" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2015" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2017" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2019" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2021" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2025" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2027" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2029" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2031" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2033" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2035" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2037" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2039" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2041" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2043" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2045" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2047" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5793,8 +5870,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5841,10 +5918,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5856,7 +5933,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>310</v>
@@ -5878,10 +5955,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5892,7 +5969,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>297</v>
@@ -5920,7 +5997,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5987,7 +6064,7 @@
         <v>300</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -6002,7 +6079,7 @@
         <v>273</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6016,7 +6093,7 @@
         <v>234</v>
       </c>
       <c r="D18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -6066,6 +6143,9 @@
       <c r="C22" t="s">
         <v>126</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5">
@@ -6078,6 +6158,9 @@
       <c r="C23" s="5" t="s">
         <v>157</v>
       </c>
+      <c r="D23" s="28" t="s">
+        <v>361</v>
+      </c>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5">
@@ -6132,10 +6215,10 @@
         <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6146,18 +6229,18 @@
         <v>56</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>340</v>
+        <v>359</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="23" t="s">
-        <v>341</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>334</v>
+        <v>358</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6168,9 +6251,9 @@
         <v>171</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>342</v>
-      </c>
-      <c r="D31" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>333</v>
       </c>
     </row>
@@ -6181,8 +6264,11 @@
       <c r="B32" t="s">
         <v>57</v>
       </c>
+      <c r="C32" s="23" t="s">
+        <v>339</v>
+      </c>
       <c r="D32" s="25" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -6194,7 +6280,7 @@
         <v>98</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -6206,7 +6292,7 @@
         <v>58</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -6227,7 +6313,7 @@
         <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>160</v>
@@ -6241,17 +6327,17 @@
       <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="23" t="s">
-        <v>359</v>
+      <c r="C37" s="10" t="s">
+        <v>341</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
       <c r="C38" s="10" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D38" t="s">
         <v>161</v>
@@ -6265,11 +6351,11 @@
       <c r="B39" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>344</v>
+      <c r="C39" s="27" t="s">
+        <v>356</v>
       </c>
       <c r="D39" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -6280,11 +6366,8 @@
       <c r="B40" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="27" t="s">
-        <v>345</v>
-      </c>
       <c r="D40" t="s">
-        <v>320</v>
+        <v>362</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -6399,7 +6482,7 @@
         <v>286</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6410,7 +6493,7 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>231</v>
@@ -6424,7 +6507,7 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>260</v>
@@ -6438,7 +6521,7 @@
         <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6448,10 +6531,13 @@
       <c r="B53" t="s">
         <v>93</v>
       </c>
+      <c r="C53" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" t="s">
-        <v>283</v>
+        <v>354</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6461,9 +6547,6 @@
       <c r="B55" t="s">
         <v>90</v>
       </c>
-      <c r="C55" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
@@ -6473,7 +6556,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6483,6 +6566,9 @@
       <c r="B57" t="s">
         <v>99</v>
       </c>
+      <c r="C57" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
@@ -6492,7 +6578,7 @@
         <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6502,9 +6588,6 @@
       <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C59" t="s">
-        <v>307</v>
-      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="8" t="s">
@@ -6513,6 +6596,9 @@
       <c r="B60" s="8" t="s">
         <v>107</v>
       </c>
+      <c r="C60" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
@@ -6521,6 +6607,9 @@
       <c r="B61" t="s">
         <v>109</v>
       </c>
+      <c r="C61" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
@@ -6980,7 +7069,7 @@
         <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -7149,18 +7238,18 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>321</v>
+      </c>
+      <c r="B163" t="s">
         <v>322</v>
-      </c>
-      <c r="B163" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -7181,7 +7270,7 @@
         <v>311</v>
       </c>
       <c r="B168" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -7213,7 +7302,7 @@
         <v>318</v>
       </c>
       <c r="B172" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -7221,12 +7310,13 @@
         <v>319</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Email pitches - created document Personalized Openings, added more emails to Marketing Components, and separated Email Template into Email Template - News and Email Template - Review. Added Team Bios to Press Kit.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="365">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -646,9 +646,6 @@
   </si>
   <si>
     <t>Tuesday (9/9)</t>
-  </si>
-  <si>
-    <t>App icon - $20</t>
   </si>
   <si>
     <t>Parse Errors (Code 1, -1011)</t>
@@ -1164,9 +1161,6 @@
     <t>Test LMU app build on another computer</t>
   </si>
   <si>
-    <t>Launch Screen - $7</t>
-  </si>
-  <si>
     <t>Autocomplete results table scroll</t>
   </si>
   <si>
@@ -1182,9 +1176,6 @@
     <t>searchResultsVC - separate VC for iOS 8</t>
   </si>
   <si>
-    <t>Look into code review tool (git pull requests)</t>
-  </si>
-  <si>
     <t>iOS 8 watch symbol</t>
   </si>
   <si>
@@ -1209,12 +1200,6 @@
     <t>Contact journalists and app review sites</t>
   </si>
   <si>
-    <t>Beta testing</t>
-  </si>
-  <si>
-    <t>Develop app video</t>
-  </si>
-  <si>
     <t>Settings/Privacy</t>
   </si>
   <si>
@@ -1225,6 +1210,24 @@
   </si>
   <si>
     <t>Web Hosting - $40 + $49</t>
+  </si>
+  <si>
+    <t>App advertising (Facebook, Pandora, YouTube)</t>
+  </si>
+  <si>
+    <t>Get app ad/video produced</t>
+  </si>
+  <si>
+    <t>Call to Action (IconShock) - $3</t>
+  </si>
+  <si>
+    <t>Launch Screen (IconShock) - $7</t>
+  </si>
+  <si>
+    <t>App icon (IconShock) - $20</t>
+  </si>
+  <si>
+    <t>Vimeo Video Hosting - $10</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1408,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2049">
+  <cellStyleXfs count="2063">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3487,7 +3504,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2049">
+  <cellStyles count="2063">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4512,6 +4529,13 @@
     <cellStyle name="Followed Hyperlink" xfId="2044" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2046" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2048" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2050" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2052" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2054" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2056" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2058" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2060" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2062" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5536,6 +5560,13 @@
     <cellStyle name="Hyperlink" xfId="2043" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2045" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2047" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2049" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2051" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2053" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2055" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2057" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2059" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2061" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5870,8 +5901,8 @@
   </sheetPr>
   <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5900,7 +5931,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -5918,10 +5949,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -5933,15 +5964,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="C6" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>120</v>
@@ -5955,10 +5986,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5969,10 +6000,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5980,10 +6011,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -5997,7 +6028,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6061,10 +6092,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -6076,10 +6107,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6090,10 +6121,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -6105,7 +6136,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
@@ -6134,7 +6165,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="13"/>
@@ -6144,7 +6175,7 @@
         <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -6159,7 +6190,7 @@
         <v>157</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -6184,7 +6215,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -6215,10 +6246,10 @@
         <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6229,18 +6260,18 @@
         <v>56</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="23" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6251,10 +6282,10 @@
         <v>171</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6264,11 +6295,11 @@
       <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>339</v>
+      <c r="C32" t="s">
+        <v>360</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -6280,7 +6311,7 @@
         <v>98</v>
       </c>
       <c r="D33" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -6292,7 +6323,7 @@
         <v>58</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -6313,7 +6344,7 @@
         <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>160</v>
@@ -6327,17 +6358,17 @@
       <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>341</v>
+      <c r="C37" s="27" t="s">
+        <v>353</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
       <c r="C38" s="10" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D38" t="s">
         <v>161</v>
@@ -6351,11 +6382,8 @@
       <c r="B39" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="27" t="s">
-        <v>356</v>
-      </c>
       <c r="D39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -6367,7 +6395,7 @@
         <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -6415,7 +6443,7 @@
         <v>138</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6426,10 +6454,10 @@
         <v>137</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E45" s="17"/>
     </row>
@@ -6438,7 +6466,7 @@
         <v>139</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E46" s="17"/>
     </row>
@@ -6450,10 +6478,10 @@
         <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>209</v>
+        <v>363</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E47" s="17"/>
     </row>
@@ -6465,10 +6493,10 @@
         <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6479,10 +6507,10 @@
         <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6493,10 +6521,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6507,10 +6535,10 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6521,7 +6549,7 @@
         <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6532,12 +6560,12 @@
         <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6547,6 +6575,9 @@
       <c r="B55" t="s">
         <v>90</v>
       </c>
+      <c r="C55" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
@@ -6556,7 +6587,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>283</v>
+        <v>364</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6566,9 +6597,6 @@
       <c r="B57" t="s">
         <v>99</v>
       </c>
-      <c r="C57" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
@@ -6578,7 +6606,7 @@
         <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6588,6 +6616,9 @@
       <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
+      <c r="C59" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="8" t="s">
@@ -6597,7 +6628,7 @@
         <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -6607,8 +6638,10 @@
       <c r="B61" t="s">
         <v>109</v>
       </c>
-      <c r="C61" t="s">
-        <v>307</v>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="C62" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -6618,6 +6651,9 @@
       <c r="B63" t="s">
         <v>111</v>
       </c>
+      <c r="C63" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
@@ -6901,7 +6937,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B104" t="s">
         <v>198</v>
@@ -6950,367 +6986,367 @@
         <v>208</v>
       </c>
       <c r="B111" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
+        <v>210</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
+        <v>215</v>
+      </c>
+      <c r="B117" t="s">
         <v>216</v>
-      </c>
-      <c r="B117" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B118" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B121" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
+        <v>221</v>
+      </c>
+      <c r="B122" t="s">
         <v>222</v>
-      </c>
-      <c r="B122" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B123" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B124" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B128" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
+        <v>243</v>
+      </c>
+      <c r="B130" t="s">
         <v>244</v>
-      </c>
-      <c r="B130" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B131" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
+        <v>246</v>
+      </c>
+      <c r="B134" t="s">
         <v>247</v>
-      </c>
-      <c r="B134" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
+        <v>248</v>
+      </c>
+      <c r="B135" t="s">
         <v>249</v>
-      </c>
-      <c r="B135" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
+        <v>250</v>
+      </c>
+      <c r="B136" t="s">
         <v>251</v>
-      </c>
-      <c r="B136" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
+        <v>254</v>
+      </c>
+      <c r="B137" t="s">
         <v>255</v>
-      </c>
-      <c r="B137" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
+        <v>252</v>
+      </c>
+      <c r="B139" t="s">
         <v>253</v>
-      </c>
-      <c r="B139" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B143" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
+        <v>262</v>
+      </c>
+      <c r="B144" t="s">
         <v>263</v>
-      </c>
-      <c r="B144" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
+        <v>264</v>
+      </c>
+      <c r="B145" t="s">
         <v>265</v>
-      </c>
-      <c r="B145" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
+        <v>266</v>
+      </c>
+      <c r="B146" t="s">
         <v>267</v>
-      </c>
-      <c r="B146" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
+        <v>275</v>
+      </c>
+      <c r="B149" t="s">
         <v>276</v>
-      </c>
-      <c r="B149" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
+        <v>277</v>
+      </c>
+      <c r="B150" t="s">
         <v>278</v>
-      </c>
-      <c r="B150" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
+        <v>286</v>
+      </c>
+      <c r="B155" t="s">
         <v>287</v>
-      </c>
-      <c r="B155" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
+        <v>288</v>
+      </c>
+      <c r="B156" t="s">
         <v>289</v>
-      </c>
-      <c r="B156" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B158" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B159" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
+        <v>294</v>
+      </c>
+      <c r="B161" t="s">
         <v>295</v>
-      </c>
-      <c r="B161" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
+        <v>320</v>
+      </c>
+      <c r="B163" t="s">
         <v>321</v>
-      </c>
-      <c r="B163" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B164" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
+        <v>307</v>
+      </c>
+      <c r="B167" t="s">
         <v>308</v>
-      </c>
-      <c r="B167" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B168" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B169" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B170" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
+        <v>315</v>
+      </c>
+      <c r="B171" t="s">
         <v>316</v>
-      </c>
-      <c r="B171" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B172" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 5 more emails to Personalized Openings and 10 more email addresses (6 general news sites) to Marketing Components. Changed text of Email Template - News to be more personal/informal (shortened/integrated app description).
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="3080" windowWidth="29220" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="39080" yWindow="0" windowWidth="29220" windowHeight="19620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="375">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1228,6 +1228,36 @@
   </si>
   <si>
     <t>Vimeo Video Hosting - $10</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Put app on VC; importing contacts from AB; friend suggestions; contactsVC alphabetized</t>
+  </si>
+  <si>
+    <t>Scrollable button label; push notif/AB permissions flow; interv. Calvin; posted to FB groups</t>
+  </si>
+  <si>
+    <t>Changed searchVC UI; new launch screens; general debugging/testing; interv. Sean</t>
+  </si>
+  <si>
+    <t>Master links; screenshots; offer/contract for Sean; submitted archive; created app video</t>
+  </si>
+  <si>
+    <t>ContactsVC - sending texts to non-users, Recents section, icons and UI; LinkedIn inMail</t>
+  </si>
+  <si>
+    <t>Refined video; helped Sean; email pitch; Dropbox press kit; emails to 19 journalists (+7)</t>
   </si>
 </sst>
 </file>
@@ -5899,10 +5929,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E173"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7349,10 +7379,57 @@
         <v>324</v>
       </c>
     </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>6</v>
+      </c>
+      <c r="B176" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>365</v>
+      </c>
+      <c r="B177" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>366</v>
+      </c>
+      <c r="B178" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>367</v>
+      </c>
+      <c r="B179" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>368</v>
+      </c>
+      <c r="B180" t="s">
+        <v>374</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
New iPhone 6 screenshots - orange gradient background with captions in Calibri.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39080" yWindow="0" windowWidth="29220" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="8620" yWindow="20" windowWidth="25600" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1257,7 +1257,7 @@
     <t>ContactsVC - sending texts to non-users, Recents section, icons and UI; LinkedIn inMail</t>
   </si>
   <si>
-    <t>Refined video; helped Sean; email pitch; Dropbox press kit; emails to 19 journalists (+7)</t>
+    <t>Finalized video; helped Sean; created press kit; emails to 19 journalists (+7 review sites)</t>
   </si>
 </sst>
 </file>
@@ -5931,7 +5931,7 @@
   </sheetPr>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finalized follow up email to journalists and updated press kit. Created document of questions for App Promo. Moved contact info for journalists / review sites / artists to new Excel spreadsheet. Added version 2.10 screenshots (larger captions) for iPhone 6.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="378">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1258,6 +1258,15 @@
   </si>
   <si>
     <t>Finalized video; helped Sean; created press kit; emails to 19 journalists (+7 review sites)</t>
+  </si>
+  <si>
+    <t>Facebook Ads -</t>
+  </si>
+  <si>
+    <t>Android Development -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KickoffLabs - </t>
   </si>
 </sst>
 </file>
@@ -1438,8 +1447,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2063">
+  <cellStyleXfs count="2075">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3534,7 +3555,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2063">
+  <cellStyles count="2075">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4566,6 +4587,12 @@
     <cellStyle name="Followed Hyperlink" xfId="2058" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2060" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2062" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2064" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2066" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2068" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2070" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2072" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2074" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5597,6 +5624,12 @@
     <cellStyle name="Hyperlink" xfId="2057" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2059" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2061" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2063" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2065" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2067" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2069" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2071" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2073" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5931,8 +5964,8 @@
   </sheetPr>
   <dimension ref="A1:E180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6627,6 +6660,9 @@
       <c r="B57" t="s">
         <v>99</v>
       </c>
+      <c r="C57" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
@@ -6636,7 +6672,7 @@
         <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>282</v>
+        <v>375</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6647,7 +6683,7 @@
         <v>105</v>
       </c>
       <c r="C59" t="s">
-        <v>284</v>
+        <v>376</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -6657,9 +6693,6 @@
       <c r="B60" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C60" t="s">
-        <v>283</v>
-      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
@@ -6668,10 +6701,13 @@
       <c r="B61" t="s">
         <v>109</v>
       </c>
+      <c r="C61" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -6682,7 +6718,7 @@
         <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -6693,23 +6729,29 @@
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>114</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>115</v>
       </c>
       <c r="B66" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>117</v>
       </c>
@@ -6717,7 +6759,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -6725,7 +6767,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -6733,7 +6775,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3">
       <c r="A71" s="15" t="s">
         <v>124</v>
       </c>
@@ -6741,7 +6783,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>125</v>
       </c>
@@ -6749,7 +6791,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>127</v>
       </c>
@@ -6757,7 +6799,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>129</v>
       </c>
@@ -6765,7 +6807,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3">
       <c r="A75" s="8" t="s">
         <v>132</v>
       </c>
@@ -6773,7 +6815,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -6781,7 +6823,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -6789,7 +6831,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>142</v>
       </c>
@@ -6797,7 +6839,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Created documents Product Hunt Post and Contest Ideas and Planning. Fixed incorrect iPhone 4 screenshot caption. Changed Facebook cover photo. Critical update for verification of international phone numbers - added instructional message to verificationVC, changed keyboard type to UIKeyboardTypePhonePad, and change code to no longer strip user input of punctuation.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="20" windowWidth="25600" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="16760" yWindow="80" windowWidth="25600" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="382">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -1267,6 +1267,18 @@
   </si>
   <si>
     <t xml:space="preserve">KickoffLabs - </t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Landing page; Facebook ads; app launch - Facebook posts and PMs; v2.05 screenshots</t>
+  </si>
+  <si>
+    <t>Signup flow bug; tested v2.05; PR agencies; YouTube stars; CPI/CPC FB ads; v2.10 screenshots</t>
   </si>
 </sst>
 </file>
@@ -5962,10 +5974,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E180"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7469,6 +7481,22 @@
         <v>374</v>
       </c>
     </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>378</v>
+      </c>
+      <c r="B181" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>379</v>
+      </c>
+      <c r="B182" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Changed contest post image to meet Facebook's 20%-text rule for ad images by downsizing logo. New Version 2.15 screenshots - lighter background and reinstanted gradient. Improvements to contestDrawing.py - sorted links datetime displayed in PST, long usernames and link titles truncated.
</commit_message>
<xml_diff>
--- a/Documents/Logs and Planning/Progress Log.xlsx
+++ b/Documents/Logs and Planning/Progress Log.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16760" yWindow="80" windowWidth="25600" windowHeight="17060" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="2460" windowWidth="29600" windowHeight="18740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
   <si>
     <t>Sunday (6/15)</t>
   </si>
@@ -501,12 +501,6 @@
     <t>Tuesday (8/19)</t>
   </si>
   <si>
-    <t>Code organization</t>
-  </si>
-  <si>
-    <t>move loadUpdatedLink, etc. to superclass</t>
-  </si>
-  <si>
     <t>Periodic data updates, data/memory usage tests, link VC song header, iTunes cell</t>
   </si>
   <si>
@@ -588,13 +582,7 @@
     <t>Song search behavior, update timer bug, set up iPhone 5s, XIB files autolayout</t>
   </si>
   <si>
-    <t>use opaque bottom bar setting in XIB files</t>
-  </si>
-  <si>
     <t>Sunday (8/31)</t>
-  </si>
-  <si>
-    <t>replace setObj, objForKey, initWithObjs w/ literals</t>
   </si>
   <si>
     <t>Monday (9/1)</t>
@@ -1043,45 +1031,9 @@
     </r>
   </si>
   <si>
-    <t>Sunday (5/24)</t>
-  </si>
-  <si>
-    <t>Updated to Xcode 6.3; resolved 2 GTL YT errors</t>
-  </si>
-  <si>
     <t>Other content sources (i.e. Soundcloud)</t>
   </si>
   <si>
-    <t>Monday (5/25)</t>
-  </si>
-  <si>
-    <t>Tuesday (5/26)</t>
-  </si>
-  <si>
-    <t>Wednesday (5/27)</t>
-  </si>
-  <si>
-    <t>Investigated FB expired token bug; reading from address book (AB); researched git</t>
-  </si>
-  <si>
-    <t>Saving AB info to Parse; integration of AB access in signup flow; list of LMU users in AB contacts</t>
-  </si>
-  <si>
-    <t>Thursday (5/28)</t>
-  </si>
-  <si>
-    <t>AB contacts as suggestions; put LMU on VC; reorg. project folder; LinkedIn post; wrote jobs page</t>
-  </si>
-  <si>
-    <t>Friday (5/29)</t>
-  </si>
-  <si>
-    <t>Saturday (5/30)</t>
-  </si>
-  <si>
-    <t>Wrote todo list; researched/practiced git for Xcode</t>
-  </si>
-  <si>
     <t>Saturday (4/3)</t>
   </si>
   <si>
@@ -1092,12 +1044,6 @@
   </si>
   <si>
     <t>Thursday (4/9)</t>
-  </si>
-  <si>
-    <t>Finished contacts VC alphab. indexing; replaced expired cert.</t>
-  </si>
-  <si>
-    <t>Pushed LMU to GitHub; SMS sending; contacts VC alphab. indexing; searched for Android devs</t>
   </si>
   <si>
     <r>
@@ -1116,15 +1062,9 @@
     </r>
   </si>
   <si>
-    <t>declare dictionary keys as constants</t>
-  </si>
-  <si>
     <t>App invites</t>
   </si>
   <si>
-    <t>move local data update functions out of Data.m</t>
-  </si>
-  <si>
     <t>Error Handling</t>
   </si>
   <si>
@@ -1134,30 +1074,18 @@
     <t>Crash/Bug Reports</t>
   </si>
   <si>
-    <t>Before Shipping</t>
-  </si>
-  <si>
     <t>Remove trunk/Examples and build/</t>
   </si>
   <si>
-    <t>Analytics - Apple, Parse</t>
-  </si>
-  <si>
     <t>Favorite links</t>
   </si>
   <si>
     <t>Marketing/Release</t>
   </si>
   <si>
-    <t>Post on news site and public forums</t>
-  </si>
-  <si>
     <t>Android Development</t>
   </si>
   <si>
-    <t>List of features/bug fixes to implement</t>
-  </si>
-  <si>
     <t>Test LMU app build on another computer</t>
   </si>
   <si>
@@ -1194,30 +1122,9 @@
     <t>Photoshop - $120</t>
   </si>
   <si>
-    <t>Build Android app on my computer</t>
-  </si>
-  <si>
-    <t>Contact journalists and app review sites</t>
-  </si>
-  <si>
     <t>Settings/Privacy</t>
   </si>
   <si>
-    <t>Use saved address book if later denied</t>
-  </si>
-  <si>
-    <t>hold song/video data in NSDictionary (subclass?)</t>
-  </si>
-  <si>
-    <t>Web Hosting - $40 + $49</t>
-  </si>
-  <si>
-    <t>App advertising (Facebook, Pandora, YouTube)</t>
-  </si>
-  <si>
-    <t>Get app ad/video produced</t>
-  </si>
-  <si>
     <t>Call to Action (IconShock) - $3</t>
   </si>
   <si>
@@ -1260,12 +1167,6 @@
     <t>Finalized video; helped Sean; created press kit; emails to 19 journalists (+7 review sites)</t>
   </si>
   <si>
-    <t>Facebook Ads -</t>
-  </si>
-  <si>
-    <t>Android Development -</t>
-  </si>
-  <si>
     <t xml:space="preserve">KickoffLabs - </t>
   </si>
   <si>
@@ -1279,6 +1180,82 @@
   </si>
   <si>
     <t>Signup flow bug; tested v2.05; PR agencies; YouTube stars; CPI/CPC FB ads; v2.10 screenshots</t>
+  </si>
+  <si>
+    <t>Post on news sites and public forums</t>
+  </si>
+  <si>
+    <t>Prepare for launch</t>
+  </si>
+  <si>
+    <t>Declare dictionary keys as constants</t>
+  </si>
+  <si>
+    <t>Move loadUpdatedLink, etc. to superclass</t>
+  </si>
+  <si>
+    <t>Move local data update functions out of Data.m</t>
+  </si>
+  <si>
+    <t>Hold song/video data in NSDictionary (subclass?)</t>
+  </si>
+  <si>
+    <t>Replace setObj, objForKey, initWithObjs w/ literals</t>
+  </si>
+  <si>
+    <t>Use opaque bottom bar setting in XIB files</t>
+  </si>
+  <si>
+    <t>Replace #define macros with constants</t>
+  </si>
+  <si>
+    <t>Promote contest</t>
+  </si>
+  <si>
+    <t>Weebly - $40 + $49</t>
+  </si>
+  <si>
+    <t>Code Organization</t>
+  </si>
+  <si>
+    <t>Configure FB pixel + Google Analytics</t>
+  </si>
+  <si>
+    <t>Don’t save address book to Parse</t>
+  </si>
+  <si>
+    <t>Production Code</t>
+  </si>
+  <si>
+    <t>Get video produced for YouTube ad</t>
+  </si>
+  <si>
+    <t>Advertise on Pinterest, Tumblr, Pandora</t>
+  </si>
+  <si>
+    <r>
+      <t>Purple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - travel</t>
+    </r>
+  </si>
+  <si>
+    <t>Update Privacy Policy / Terms in app</t>
+  </si>
+  <si>
+    <t>Create custom landing page</t>
+  </si>
+  <si>
+    <t>Facebook Ads - $119.61</t>
+  </si>
+  <si>
+    <t>Android Development - $2250</t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1443,12 +1420,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC4D79B"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1459,8 +1430,96 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2075">
+  <cellStyleXfs count="2163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3564,10 +3623,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2075">
+  <cellStyles count="2163">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4605,6 +4664,50 @@
     <cellStyle name="Followed Hyperlink" xfId="2070" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2072" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2074" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2076" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2078" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2080" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2082" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2084" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2086" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2088" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2090" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2092" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2094" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2096" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2098" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2162" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5642,6 +5745,50 @@
     <cellStyle name="Hyperlink" xfId="2069" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2071" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2073" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2075" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2077" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2079" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2081" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2083" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2085" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2087" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2089" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2091" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2093" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2095" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2097" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2099" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2161" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5974,10 +6121,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6006,7 +6153,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>44</v>
@@ -6023,11 +6170,11 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>342</v>
+      <c r="C4" s="25" t="s">
+        <v>297</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="E4" s="5"/>
     </row>
@@ -6039,15 +6186,15 @@
         <v>26</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="C6" s="25" t="s">
-        <v>301</v>
+      <c r="C6" s="26" t="s">
+        <v>318</v>
       </c>
       <c r="D6" s="26" t="s">
         <v>120</v>
@@ -6061,10 +6208,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6075,10 +6222,10 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6086,10 +6233,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -6103,7 +6250,7 @@
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6137,7 +6284,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E13" s="5"/>
     </row>
@@ -6167,10 +6314,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -6182,10 +6329,10 @@
         <v>29</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6196,10 +6343,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -6211,7 +6358,7 @@
         <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D19" t="s">
         <v>95</v>
@@ -6240,7 +6387,7 @@
         <v>30</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="13"/>
@@ -6250,7 +6397,7 @@
         <v>126</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>355</v>
+        <v>329</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -6264,8 +6411,8 @@
       <c r="C23" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D23" s="28" t="s">
-        <v>356</v>
+      <c r="D23" s="27" t="s">
+        <v>362</v>
       </c>
       <c r="E23" s="11"/>
     </row>
@@ -6279,7 +6426,9 @@
       <c r="C24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="6"/>
+      <c r="D24" s="27" t="s">
+        <v>367</v>
+      </c>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5">
@@ -6290,7 +6439,7 @@
         <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E25" s="12"/>
     </row>
@@ -6302,7 +6451,7 @@
         <v>96</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6321,10 +6470,10 @@
         <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>333</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6335,18 +6484,18 @@
         <v>56</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="C30" s="23" t="s">
-        <v>338</v>
+        <v>368</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6354,13 +6503,13 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>359</v>
+        <v>169</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>349</v>
       </c>
       <c r="D31" s="25" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6370,11 +6519,11 @@
       <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C32" t="s">
-        <v>360</v>
+      <c r="C32" s="10" t="s">
+        <v>361</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="E32" s="11"/>
     </row>
@@ -6385,8 +6534,11 @@
       <c r="B33" t="s">
         <v>98</v>
       </c>
+      <c r="C33" s="25" t="s">
+        <v>364</v>
+      </c>
       <c r="D33" s="25" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="E33" s="11"/>
     </row>
@@ -6397,8 +6549,8 @@
       <c r="B34" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="25" t="s">
-        <v>330</v>
+      <c r="C34" s="25" t="s">
+        <v>365</v>
       </c>
       <c r="E34" s="12"/>
     </row>
@@ -6419,10 +6571,10 @@
         <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="E36" s="11"/>
     </row>
@@ -6433,20 +6585,17 @@
       <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>353</v>
+      <c r="C37" s="23" t="s">
+        <v>350</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>327</v>
+        <v>351</v>
       </c>
       <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="C38" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="D38" t="s">
-        <v>161</v>
+      <c r="D38" s="25" t="s">
+        <v>357</v>
       </c>
       <c r="E38" s="12"/>
     </row>
@@ -6458,7 +6607,7 @@
         <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="E39" s="17"/>
     </row>
@@ -6470,7 +6619,7 @@
         <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -6482,7 +6631,7 @@
         <v>94</v>
       </c>
       <c r="D41" t="s">
-        <v>191</v>
+        <v>354</v>
       </c>
       <c r="E41" s="11"/>
     </row>
@@ -6494,7 +6643,7 @@
         <v>69</v>
       </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>355</v>
       </c>
       <c r="E42" s="11"/>
     </row>
@@ -6505,6 +6654,9 @@
       <c r="B43" s="15" t="s">
         <v>73</v>
       </c>
+      <c r="D43" t="s">
+        <v>356</v>
+      </c>
       <c r="E43" s="17"/>
     </row>
     <row r="44" spans="1:5">
@@ -6514,12 +6666,6 @@
       <c r="B44" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
@@ -6528,20 +6674,20 @@
       <c r="B45" t="s">
         <v>137</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>229</v>
+      <c r="C45" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="E45" s="17"/>
     </row>
     <row r="46" spans="1:5">
       <c r="C46" s="7" t="s">
-        <v>139</v>
+        <v>294</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E46" s="17"/>
     </row>
@@ -6552,11 +6698,11 @@
       <c r="B47" t="s">
         <v>76</v>
       </c>
-      <c r="C47" t="s">
-        <v>363</v>
+      <c r="C47" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E47" s="17"/>
     </row>
@@ -6568,10 +6714,10 @@
         <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>228</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>239</v>
+        <v>332</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -6582,10 +6728,10 @@
         <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>285</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>346</v>
+        <v>224</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -6596,10 +6742,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>358</v>
+        <v>281</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>230</v>
+        <v>322</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -6610,10 +6756,10 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>297</v>
+        <v>359</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>259</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -6624,7 +6770,10 @@
         <v>102</v>
       </c>
       <c r="C52" t="s">
-        <v>362</v>
+        <v>293</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -6635,12 +6784,12 @@
         <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="C54" t="s">
-        <v>351</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -6651,7 +6800,7 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>361</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -6662,7 +6811,7 @@
         <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>364</v>
+        <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -6673,7 +6822,7 @@
         <v>99</v>
       </c>
       <c r="C57" t="s">
-        <v>377</v>
+        <v>333</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -6684,7 +6833,7 @@
         <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -6694,8 +6843,8 @@
       <c r="B59" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C59" t="s">
-        <v>376</v>
+      <c r="C59" s="22" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -6705,6 +6854,9 @@
       <c r="B60" s="8" t="s">
         <v>107</v>
       </c>
+      <c r="C60" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
@@ -6713,13 +6865,10 @@
       <c r="B61" t="s">
         <v>109</v>
       </c>
-      <c r="C61" t="s">
-        <v>282</v>
-      </c>
     </row>
     <row r="62" spans="1:4">
       <c r="C62" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -6730,7 +6879,7 @@
         <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -6740,6 +6889,9 @@
       <c r="B64" t="s">
         <v>113</v>
       </c>
+      <c r="C64" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
@@ -6748,9 +6900,6 @@
       <c r="B65" t="s">
         <v>116</v>
       </c>
-      <c r="C65" t="s">
-        <v>305</v>
-      </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -6760,7 +6909,7 @@
         <v>130</v>
       </c>
       <c r="C66" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -6770,6 +6919,9 @@
       <c r="B67" t="s">
         <v>118</v>
       </c>
+      <c r="C67" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
@@ -6778,6 +6930,9 @@
       <c r="B68" t="s">
         <v>123</v>
       </c>
+      <c r="C68" s="28" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
@@ -6832,7 +6987,7 @@
         <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -6840,7 +6995,7 @@
         <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -6904,602 +7059,547 @@
         <v>159</v>
       </c>
       <c r="B87" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
+        <v>171</v>
+      </c>
+      <c r="B93" t="s">
         <v>173</v>
-      </c>
-      <c r="B93" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B96" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B97" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B98" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B101" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B103" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B104" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
+        <v>199</v>
+      </c>
+      <c r="B107" t="s">
         <v>203</v>
-      </c>
-      <c r="B107" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="24" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B108" s="21"/>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B109" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
+        <v>204</v>
+      </c>
+      <c r="B111" t="s">
         <v>208</v>
-      </c>
-      <c r="B111" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B117" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B118" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B121" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B122" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B123" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B124" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B125" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B128" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B130" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B131" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B135" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B136" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B137" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B139" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="22" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B143" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B145" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B146" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B149" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B150" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B153" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B155" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B156" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B158" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B159" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B161" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="B163" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="B164" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>307</v>
+        <v>7</v>
       </c>
       <c r="B167" t="s">
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>310</v>
+        <v>6</v>
       </c>
       <c r="B168" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="B169" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="B170" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
       <c r="B171" t="s">
-        <v>316</v>
+        <v>341</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="B172" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
     </row>
     <row r="173" spans="1:2">
-      <c r="A173" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="B173" s="8" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2">
-      <c r="A175" t="s">
-        <v>7</v>
-      </c>
-      <c r="B175" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2">
-      <c r="A176" t="s">
-        <v>6</v>
-      </c>
-      <c r="B176" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="A177" t="s">
-        <v>365</v>
-      </c>
-      <c r="B177" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
-      <c r="A178" t="s">
-        <v>366</v>
-      </c>
-      <c r="B178" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
-      <c r="A179" t="s">
-        <v>367</v>
-      </c>
-      <c r="B179" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
-      <c r="A180" t="s">
-        <v>368</v>
-      </c>
-      <c r="B180" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
-      <c r="A181" t="s">
-        <v>378</v>
-      </c>
-      <c r="B181" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
-      <c r="A182" t="s">
-        <v>379</v>
-      </c>
-      <c r="B182" t="s">
-        <v>381</v>
+      <c r="A173" t="s">
+        <v>345</v>
+      </c>
+      <c r="B173" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>